<commit_message>
first sweep cleaning data columns to conform to specs--done by chase
</commit_message>
<xml_diff>
--- a/bioSample/bioSample_hbrown_05.20.19.xlsx
+++ b/bioSample/bioSample_hbrown_05.20.19.xlsx
@@ -64,10 +64,10 @@
     <t xml:space="preserve">H.BROWN</t>
   </si>
   <si>
-    <t xml:space="preserve">Environmental Perturbation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">KN 99 alpha</t>
+    <t xml:space="preserve">Environmental_Perturbation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KN 99_alpha</t>
   </si>
   <si>
     <t xml:space="preserve">CNAG_00000</t>
@@ -207,7 +207,7 @@
   <dimension ref="A1:Z27"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2:B27"/>
+      <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2:F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
added template and corrected metadata files to all use the same format
</commit_message>
<xml_diff>
--- a/bioSample/bioSample_hbrown_05.20.19.xlsx
+++ b/bioSample/bioSample_hbrown_05.20.19.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hollybrown/database_files/bioSample/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54681695-F20A-014F-AA9F-2C7A8DD5297E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0991F2B0-5DD2-7642-BF16-3DC4E561C47C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="20760" windowHeight="13240" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -96,7 +96,7 @@
     <t>YPD.37C.cAMP</t>
   </si>
   <si>
-    <t>KN 99alpha</t>
+    <t>KN99alpha</t>
   </si>
 </sst>
 </file>

</xml_diff>